<commit_message>
Update task excel, structure.
</commit_message>
<xml_diff>
--- a/document/Task.xlsx
+++ b/document/Task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>No</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Trí</t>
   </si>
   <si>
-    <t>Hạnh</t>
-  </si>
-  <si>
     <t>Design page sign in by Angular</t>
   </si>
   <si>
@@ -57,16 +54,25 @@
     <t>Integrate JWT into Spring Boot</t>
   </si>
   <si>
-    <t>Build api to save new account &amp; design add new account page</t>
-  </si>
-  <si>
-    <t>Design page view list account &amp; detail account</t>
-  </si>
-  <si>
-    <t>Build api to update and delete account</t>
-  </si>
-  <si>
-    <t>Sign up with google, facebook. Validate data input</t>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Hạnh &amp; Trang</t>
+  </si>
+  <si>
+    <t>Update db</t>
+  </si>
+  <si>
+    <t>Ngân &amp; Trí</t>
+  </si>
+  <si>
+    <t>Vân</t>
+  </si>
+  <si>
+    <t>Design ui &amp; api for expense &amp; income</t>
+  </si>
+  <si>
+    <t>Design ui &amp; api for account</t>
   </si>
 </sst>
 </file>
@@ -74,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -107,7 +113,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,19 +415,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,13 +448,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -461,12 +472,12 @@
         <v>43228</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -481,12 +492,12 @@
         <v>43228</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -499,12 +510,12 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -516,16 +527,19 @@
       <c r="F5" s="1">
         <v>43229</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>43228</v>
@@ -534,38 +548,28 @@
       <c r="F6" s="1">
         <v>43229</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <v>43228</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <v>43229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>43228</v>
-      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>

</xml_diff>